<commit_message>
Atualização dos casos de testes. CT-08.xlsx
</commit_message>
<xml_diff>
--- a/Software para Deficientes Visuais/Casos de Teste/CT-08.xlsx
+++ b/Software para Deficientes Visuais/Casos de Teste/CT-08.xlsx
@@ -142,9 +142,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,9 +187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -203,6 +198,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -500,17 +498,17 @@
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="5"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
     <col min="4" max="4" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,7 +534,7 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -544,86 +542,86 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -640,16 +638,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>